<commit_message>
create postgres table & insert into table with auto seq & read xls columns file
</commit_message>
<xml_diff>
--- a/indicadores.xlsx
+++ b/indicadores.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.silva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\cubes\csvParser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="indicadores" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>DICOFRE</t>
   </si>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -316,6 +316,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -351,6 +368,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -503,964 +537,1021 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1024" width="15"/>
+    <col min="2" max="1025" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1991</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>110.26</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>89.048638999999994</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>102.128159</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>14497</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>6560</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>162.79866899999999</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>64.233018999999999</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>60.596794000000003</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>91.365729000000002</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>239.237078</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>71.799351000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1991</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>98.58</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.99</v>
-      </c>
-      <c r="G3">
-        <v>98.581777000000002</v>
       </c>
       <c r="H3">
         <v>98.581777000000002</v>
       </c>
       <c r="I3">
+        <v>98.581777000000002</v>
+      </c>
+      <c r="J3">
         <v>16879</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>5517</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>171.21825699999999</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>55.96369</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>84.207250999999999</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>94.117816000000005</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>200.44592</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>58.618018999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1991</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>131.99</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.32</v>
-      </c>
-      <c r="G4">
-        <v>131.985783</v>
       </c>
       <c r="H4">
         <v>131.985783</v>
       </c>
       <c r="I4">
+        <v>131.985783</v>
+      </c>
+      <c r="J4">
         <v>4378</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3570</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>33.170239000000002</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>27.048368</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>86.204750000000004</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>119.232236</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>50.786064000000003</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>29.941566999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1991</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>408.4</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>4.08</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>370.40634999999997</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>451.09243900000001</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>16231</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>8708</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>43.819443</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>19.304247</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>203.545323</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>295.69206400000002</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>79.741454000000004</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>29.449556000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1991</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>567.23</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>5.67</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>429.61722600000002</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>489.82979599999999</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>20800</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>9513</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>48.415191</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>19.421032</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>305.50782400000003</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>340.300005</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>68.083363000000006</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>27.954744999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1991</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>356.92</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>3.57</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>185.67546200000001</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>241.40911700000001</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>9041</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>4228</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>48.692487</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>17.513836999999999</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>146.682951</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>190.33079000000001</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>61.636339</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>22.213957000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1991</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>141.16999999999999</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1.41</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>48.161523000000003</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>76.468748000000005</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>3419</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2785</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>70.990279999999998</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>36.420107000000002</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>30.835822</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>57.78398</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>110.877538</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>48.196748999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1991</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>363.25</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3.63</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>458.05102799999997</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>579.89101800000003</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>26267</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>12258</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>57.345139000000003</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>21.138455</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>100.714528</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>164.076054</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>260.80646400000001</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>74.709255999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1991</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>556.46</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>5.56</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>83.686893999999995</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>130.145726</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1596</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1088</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>19.071086999999999</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>8.3598599999999994</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>132.40897899999999</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>154.026003</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>12.053563</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>7.0637420000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1991</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
       <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>448.19</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4.4800000000000004</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>132.88516100000001</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>159.506528</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>9818</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>4668</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>73.883342999999996</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>29.265260000000001</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>139.27549099999999</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>134.88883100000001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>70.493379000000004</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>34.606274999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1991</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
       <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>643.20000000000005</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>6.43</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>94.250760999999997</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>178.556681</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>15511</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>8360</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>164.57161500000001</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>46.819867000000002</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>279.34545400000002</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>356.40939600000002</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>55.526229999999998</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>23.456171999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1991</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
       <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>751.55</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>7.52</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>96.085802000000001</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>285.77498400000002</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>15645</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>8836</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>162.82322400000001</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>30.919430999999999</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>322.70063199999998</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>430.79464100000001</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>48.481467000000002</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>20.510933000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1991</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>3281.5</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>32.82</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>550.34681699999999</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>726.86566400000004</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>19636</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>13071</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>35.679319999999997</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>17.982690000000002</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>568.25695199999996</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>679.83069999999998</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>34.554791000000002</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>19.226845999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1991</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1512.91</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>15.13</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>329.39085599999999</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>333.09633200000002</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>4236</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>2097</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>12.860101999999999</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>6.2954759999999998</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>169.191518</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>226.93308300000001</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>25.036715999999998</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>9.2406089999999992</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1991</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
       <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>1327.89</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>13.28</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>134.098332</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>229.43694099999999</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>3403</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1850</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>25.376899999999999</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>8.0632180000000009</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>99.139906999999994</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>309.26165500000002</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>34.325229</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>5.9819899999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1991</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
       <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
         <v>19</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>1162.9100000000001</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>11.63</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>86.876088999999993</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>102.141959</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>2690</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>1403</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>30.963640999999999</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>13.735785</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>88.907904000000002</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>117.95019499999999</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>30.256028000000001</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>11.894850999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1991</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
       <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
         <v>19</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1652.21</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>16.52</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>87.081734999999995</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>206.93813900000001</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>3164</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>1511</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>36.333680999999999</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>7.3016990000000002</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>169.812083</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>262.398706</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>18.632361</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>5.758413</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1991</v>
+      </c>
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
       <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
         <v>19</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>3396.9</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>33.97</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>48.522914</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>148.66862900000001</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>4932</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>2243</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>101.642701</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>15.087244999999999</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>152.22163499999999</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>368.47706299999999</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>32.400125000000003</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>6.0872169999999999</v>
       </c>
     </row>
@@ -1473,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1694,5 +1785,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code refactoring to main->parse2db & 3 classes
</commit_message>
<xml_diff>
--- a/indicadores.xlsx
+++ b/indicadores.xlsx
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>